<commit_message>
refact delete by update person
</commit_message>
<xml_diff>
--- a/Login.xlsx
+++ b/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,47 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Hash-Algo</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>authentication</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>tinyInt/bool</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>SecureWord</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53,7 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,7 +110,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +155,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +190,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +372,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>